<commit_message>
clean up unused imports
</commit_message>
<xml_diff>
--- a/src/python/comp230/sample_db.xlsx
+++ b/src/python/comp230/sample_db.xlsx
@@ -808,7 +808,7 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="16">
+  <dataValidations count="24">
     <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Invalid Entry" error="Duplicate entry" type="custom">
       <formula1>COUNTIF(A:A, A2)&lt;=1</formula1>
     </dataValidation>
@@ -821,6 +821,26 @@
     </dataValidation>
     <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Invalid Entry" error="Duplicate entry" type="custom">
       <formula1>COUNTIF(A:A, A2)&lt;=1</formula1>
+    </dataValidation>
+    <dataValidation sqref="B2:B1048576 A2:A1048576 C2:C1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Invalid Entry" error="Need to enter data of type: whole. And its value needs to: greaterThanOrEqual 0" type="whole" operator="greaterThanOrEqual">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation sqref="C2:C1048576 E2:E1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Invalid Entry" error="Need to enter data of type: date. And its value needs to: None None" type="date"/>
+    <dataValidation sqref="D2:D1048576 C2:C1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Invalid Entry" error="Need to enter data of type: decimal. And its value needs to: greaterThanOrEqual 0" type="decimal" operator="greaterThanOrEqual">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Invalid Entry" error="Duplicate entry" type="custom">
+      <formula1>=countif(A:A, A2)&lt;=1</formula1>
+    </dataValidation>
+    <dataValidation sqref="B2:B1048576 A2:A1048576 C2:C1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Invalid Entry" error="Need to enter data of type: whole. And its value needs to: greaterThanOrEqual 0" type="whole" operator="greaterThanOrEqual">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation sqref="C2:C1048576 E2:E1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Invalid Entry" error="Need to enter data of type: date. And its value needs to: None None" type="date"/>
+    <dataValidation sqref="D2:D1048576 C2:C1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Invalid Entry" error="Need to enter data of type: decimal. And its value needs to: greaterThanOrEqual 0" type="decimal" operator="greaterThanOrEqual">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Invalid Entry" error="Duplicate entry" type="custom">
+      <formula1>=countif(A:A, A2)&lt;=1</formula1>
     </dataValidation>
     <dataValidation sqref="B2:B1048576 A2:A1048576 C2:C1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Invalid Entry" error="Need to enter data of type: whole. And its value needs to: greaterThanOrEqual 0" type="whole" operator="greaterThanOrEqual">
       <formula1>0</formula1>
@@ -1260,7 +1280,25 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="12">
+  <dataValidations count="18">
+    <dataValidation sqref="B2:B1048576 A2:A1048576 C2:C1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Invalid Entry" error="Need to enter data of type: whole. And its value needs to: greaterThanOrEqual 0" type="whole" operator="greaterThanOrEqual">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation sqref="B2:B1048576 A2:A1048576 C2:C1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Invalid Entry" error="Need to enter data of type: whole. And its value needs to: greaterThanOrEqual 0" type="whole" operator="greaterThanOrEqual">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation sqref="B2:B1048576 A2:A1048576 C2:C1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Invalid Entry" error="Need to enter data of type: whole. And its value needs to: greaterThanOrEqual 0" type="whole" operator="greaterThanOrEqual">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation sqref="B2:B1048576 A2:A1048576 C2:C1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Invalid Entry" error="Need to enter data of type: whole. And its value needs to: greaterThanOrEqual 0" type="whole" operator="greaterThanOrEqual">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation sqref="B2:B1048576 A2:A1048576 C2:C1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Invalid Entry" error="Need to enter data of type: whole. And its value needs to: greaterThanOrEqual 0" type="whole" operator="greaterThanOrEqual">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation sqref="B2:B1048576 A2:A1048576 C2:C1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Invalid Entry" error="Need to enter data of type: whole. And its value needs to: greaterThanOrEqual 0" type="whole" operator="greaterThanOrEqual">
+      <formula1>0</formula1>
+    </dataValidation>
     <dataValidation sqref="B2:B1048576 A2:A1048576 C2:C1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Invalid Entry" error="Need to enter data of type: whole. And its value needs to: greaterThanOrEqual 0" type="whole" operator="greaterThanOrEqual">
       <formula1>0</formula1>
     </dataValidation>
@@ -1739,7 +1777,7 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="24">
+  <dataValidations count="36">
     <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Invalid Entry" error="Duplicate entry" type="custom">
       <formula1>COUNTIF(A:A, A2)&lt;=1</formula1>
     </dataValidation>
@@ -1771,6 +1809,40 @@
     </dataValidation>
     <dataValidation sqref="C2:C1048576 E2:E1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Invalid Entry" error="Need to enter data of type: date. And its value needs to: None None" type="date"/>
     <dataValidation sqref="F2:F1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Invalid Entry" error="Need to enter data of type: whole. And its value needs to: between 0 and 1" type="whole">
+      <formula1>0</formula1>
+      <formula2>1</formula2>
+    </dataValidation>
+    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Invalid Entry" error="Duplicate entry" type="custom">
+      <formula1>=countif(A:A, A2)&lt;=1</formula1>
+    </dataValidation>
+    <dataValidation sqref="B2:B1048576 C2:C1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Invalid Entry" error="Need to enter data of type: textLength. And its value needs to: lessThanOrEqual 20" type="textLength" operator="lessThanOrEqual">
+      <formula1>20</formula1>
+    </dataValidation>
+    <dataValidation sqref="B2:B1048576 C2:C1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Invalid Entry" error="Need to enter data of type: textLength. And its value needs to: lessThanOrEqual 20" type="textLength" operator="lessThanOrEqual">
+      <formula1>20</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2:D1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Invalid Entry" error="Need to enter data of type: textLength. And its value needs to: lessThanOrEqual 50" type="textLength" operator="lessThanOrEqual">
+      <formula1>50</formula1>
+    </dataValidation>
+    <dataValidation sqref="C2:C1048576 E2:E1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Invalid Entry" error="Need to enter data of type: date. And its value needs to: None None" type="date"/>
+    <dataValidation sqref="F2:F1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Invalid Entry" error="Need to enter data of type: whole. And its value needs to: between 0 and 1" type="whole" operator="between">
+      <formula1>0</formula1>
+      <formula2>1</formula2>
+    </dataValidation>
+    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Invalid Entry" error="Duplicate entry" type="custom">
+      <formula1>=countif(A:A, A2)&lt;=1</formula1>
+    </dataValidation>
+    <dataValidation sqref="B2:B1048576 C2:C1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Invalid Entry" error="Need to enter data of type: textLength. And its value needs to: lessThanOrEqual 20" type="textLength" operator="lessThanOrEqual">
+      <formula1>20</formula1>
+    </dataValidation>
+    <dataValidation sqref="B2:B1048576 C2:C1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Invalid Entry" error="Need to enter data of type: textLength. And its value needs to: lessThanOrEqual 20" type="textLength" operator="lessThanOrEqual">
+      <formula1>20</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2:D1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Invalid Entry" error="Need to enter data of type: textLength. And its value needs to: lessThanOrEqual 50" type="textLength" operator="lessThanOrEqual">
+      <formula1>50</formula1>
+    </dataValidation>
+    <dataValidation sqref="C2:C1048576 E2:E1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Invalid Entry" error="Need to enter data of type: date. And its value needs to: None None" type="date"/>
+    <dataValidation sqref="F2:F1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Invalid Entry" error="Need to enter data of type: whole. And its value needs to: between 0 and 1" type="whole" operator="between">
       <formula1>0</formula1>
       <formula2>1</formula2>
     </dataValidation>
@@ -1968,7 +2040,7 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="12">
+  <dataValidations count="18">
     <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Invalid Entry" error="Duplicate entry" type="custom">
       <formula1>COUNTIF(A:A, A2)&lt;=1</formula1>
     </dataValidation>
@@ -1980,6 +2052,24 @@
     </dataValidation>
     <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Invalid Entry" error="Duplicate entry" type="custom">
       <formula1>COUNTIF(A:A, A2)&lt;=1</formula1>
+    </dataValidation>
+    <dataValidation sqref="B2:B1048576 C2:C1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Invalid Entry" error="Need to enter data of type: textLength. And its value needs to: lessThanOrEqual 20" type="textLength" operator="lessThanOrEqual">
+      <formula1>20</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2:D1048576 C2:C1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Invalid Entry" error="Need to enter data of type: decimal. And its value needs to: greaterThanOrEqual 0" type="decimal" operator="greaterThanOrEqual">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Invalid Entry" error="Duplicate entry" type="custom">
+      <formula1>=countif(A:A, A2)&lt;=1</formula1>
+    </dataValidation>
+    <dataValidation sqref="B2:B1048576 C2:C1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Invalid Entry" error="Need to enter data of type: textLength. And its value needs to: lessThanOrEqual 20" type="textLength" operator="lessThanOrEqual">
+      <formula1>20</formula1>
+    </dataValidation>
+    <dataValidation sqref="D2:D1048576 C2:C1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Invalid Entry" error="Need to enter data of type: decimal. And its value needs to: greaterThanOrEqual 0" type="decimal" operator="greaterThanOrEqual">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation sqref="A2:A1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Invalid Entry" error="Duplicate entry" type="custom">
+      <formula1>=countif(A:A, A2)&lt;=1</formula1>
     </dataValidation>
     <dataValidation sqref="B2:B1048576 C2:C1048576" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Invalid Entry" error="Need to enter data of type: textLength. And its value needs to: lessThanOrEqual 20" type="textLength" operator="lessThanOrEqual">
       <formula1>20</formula1>

</xml_diff>